<commit_message>
Removed online cost data
</commit_message>
<xml_diff>
--- a/Deck_cost.xlsx
+++ b/Deck_cost.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://informaplc-my.sharepoint.com/personal/brian_mackenzie_informa_com/Documents/Documents/GitHub/Modern-Cost/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MackenzieB\Modern-Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{E798A65C-45E7-4203-83E6-E54DA41901EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{47247A4E-ACB4-4DCF-89A0-BB1B9146115B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F48DE30-BCB1-4789-B6BB-430942B83081}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3A466C81-8ADB-4721-8983-0E8C39BED239}"/>
   </bookViews>
@@ -412,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E2E044-A947-4841-B752-CB22CAC72FC7}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>2021</v>
       </c>
@@ -442,32 +442,26 @@
       <c r="G1" s="1">
         <v>2015</v>
       </c>
-      <c r="H1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2013</v>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>649</v>
       </c>
@@ -489,37 +483,31 @@
       <c r="G2">
         <v>367</v>
       </c>
-      <c r="H2">
-        <v>217</v>
-      </c>
       <c r="I2">
-        <v>739</v>
-      </c>
-      <c r="K2">
         <v>2021</v>
       </c>
-      <c r="L2">
+      <c r="J2">
         <f>AVERAGE(A2:A23)</f>
         <v>1046</v>
       </c>
-      <c r="M2">
+      <c r="K2">
         <f>MEDIAN(A2:A23)</f>
         <v>1084.5</v>
       </c>
-      <c r="N2">
+      <c r="L2">
         <f>MAX(A2:A23)</f>
         <v>1812</v>
       </c>
-      <c r="O2">
+      <c r="M2">
         <f>MIN(A2:A23)</f>
         <v>373</v>
       </c>
-      <c r="P2">
+      <c r="N2">
         <f>COUNT(A2:A23)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>479</v>
       </c>
@@ -541,37 +529,31 @@
       <c r="G3">
         <v>1115</v>
       </c>
-      <c r="H3">
-        <v>748</v>
-      </c>
       <c r="I3">
-        <v>58</v>
-      </c>
-      <c r="K3">
         <v>2020</v>
       </c>
-      <c r="L3">
+      <c r="J3">
         <f>AVERAGE(B2:B32)</f>
         <v>718.32258064516134</v>
       </c>
-      <c r="M3">
+      <c r="K3">
         <f>MEDIAN(B2:B32)</f>
         <v>659</v>
       </c>
-      <c r="N3">
+      <c r="L3">
         <f>MAX(B2:B32)</f>
         <v>1585</v>
       </c>
-      <c r="O3">
+      <c r="M3">
         <f>MIN(B2:B32)</f>
         <v>224</v>
       </c>
-      <c r="P3">
+      <c r="N3">
         <f>COUNT(B2:B32)</f>
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1130</v>
       </c>
@@ -593,37 +575,31 @@
       <c r="G4">
         <v>1094</v>
       </c>
-      <c r="H4">
-        <v>225</v>
-      </c>
       <c r="I4">
-        <v>184</v>
-      </c>
-      <c r="K4">
         <v>2019</v>
       </c>
-      <c r="L4">
+      <c r="J4">
         <f>AVERAGE(C2:C22)</f>
         <v>856.61904761904759</v>
       </c>
-      <c r="M4">
+      <c r="K4">
         <f>MEDIAN(C2:C22)</f>
         <v>821</v>
       </c>
-      <c r="N4">
+      <c r="L4">
         <f>MAX(C2:C22)</f>
         <v>1707</v>
       </c>
-      <c r="O4">
+      <c r="M4">
         <f>MIN(C2:C22)</f>
         <v>284</v>
       </c>
-      <c r="P4">
+      <c r="N4">
         <f>COUNT(C2:C22)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>648</v>
       </c>
@@ -645,37 +621,31 @@
       <c r="G5">
         <v>891</v>
       </c>
-      <c r="H5">
-        <v>453</v>
-      </c>
       <c r="I5">
-        <v>472</v>
-      </c>
-      <c r="K5">
         <v>2018</v>
       </c>
-      <c r="L5">
+      <c r="J5">
         <f>AVERAGE(D2:D25)</f>
         <v>852.20833333333337</v>
       </c>
-      <c r="M5">
+      <c r="K5">
         <f>MEDIAN(D2:D25)</f>
         <v>755.5</v>
       </c>
-      <c r="N5">
+      <c r="L5">
         <f>MAX(D2:D25)</f>
         <v>1684</v>
       </c>
-      <c r="O5">
+      <c r="M5">
         <f>MIN(D2:D25)</f>
         <v>291</v>
       </c>
-      <c r="P5">
+      <c r="N5">
         <f>COUNT(D2:D25)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1137</v>
       </c>
@@ -697,37 +667,31 @@
       <c r="G6">
         <v>694</v>
       </c>
-      <c r="H6">
-        <v>303</v>
-      </c>
       <c r="I6">
-        <v>51</v>
-      </c>
-      <c r="K6">
         <v>2017</v>
       </c>
-      <c r="L6">
+      <c r="J6">
         <f>AVERAGE(E2:E18)</f>
         <v>801</v>
       </c>
-      <c r="M6">
+      <c r="K6">
         <f>MEDIAN(E2:E18)</f>
         <v>811</v>
       </c>
-      <c r="N6">
+      <c r="L6">
         <f>MAX(E2:E18)</f>
         <v>1591</v>
       </c>
-      <c r="O6">
+      <c r="M6">
         <f>MIN(E2:E18)</f>
         <v>426</v>
       </c>
-      <c r="P6">
+      <c r="N6">
         <f>COUNT(E2:E18)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>373</v>
       </c>
@@ -749,37 +713,31 @@
       <c r="G7">
         <v>1303</v>
       </c>
-      <c r="H7">
-        <v>653</v>
-      </c>
       <c r="I7">
-        <v>395</v>
-      </c>
-      <c r="K7">
         <v>2016</v>
       </c>
-      <c r="L7">
+      <c r="J7">
         <f>AVERAGE(F2:F27)</f>
         <v>847.07692307692309</v>
       </c>
-      <c r="M7">
+      <c r="K7">
         <f>MEDIAN(F2:F27)</f>
         <v>770</v>
       </c>
-      <c r="N7">
+      <c r="L7">
         <f>MAX(F2:F27)</f>
         <v>2015</v>
       </c>
-      <c r="O7">
+      <c r="M7">
         <f>MIN(F2:F27)</f>
         <v>288</v>
       </c>
-      <c r="P7">
+      <c r="N7">
         <f>COUNT(F2:F27)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1229</v>
       </c>
@@ -801,37 +759,31 @@
       <c r="G8">
         <v>516</v>
       </c>
-      <c r="H8">
-        <v>62</v>
-      </c>
       <c r="I8">
-        <v>174</v>
-      </c>
-      <c r="K8">
         <v>2015</v>
       </c>
-      <c r="L8">
+      <c r="J8">
         <f>AVERAGE(G2:G23)</f>
         <v>881.68181818181813</v>
       </c>
-      <c r="M8">
+      <c r="K8">
         <f>MEDIAN(G2:G23)</f>
         <v>785.5</v>
       </c>
-      <c r="N8">
+      <c r="L8">
         <f>MAX(G2:G23)</f>
         <v>1858</v>
       </c>
-      <c r="O8">
+      <c r="M8">
         <f>MIN(G2:G23)</f>
         <v>367</v>
       </c>
-      <c r="P8">
+      <c r="N8">
         <f>COUNT(G2:G23)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>685</v>
       </c>
@@ -853,37 +805,8 @@
       <c r="G9">
         <v>542</v>
       </c>
-      <c r="H9">
-        <v>192</v>
-      </c>
-      <c r="I9">
-        <v>225</v>
-      </c>
-      <c r="K9">
-        <v>2014</v>
-      </c>
-      <c r="L9">
-        <f>AVERAGE(H2:H25)</f>
-        <v>468.45833333333331</v>
-      </c>
-      <c r="M9">
-        <f>MEDIAN(H2:H25)</f>
-        <v>421</v>
-      </c>
-      <c r="N9">
-        <f>MAX(H2:H25)</f>
-        <v>1221</v>
-      </c>
-      <c r="O9">
-        <f>MIN(H2:H25)</f>
-        <v>62</v>
-      </c>
-      <c r="P9">
-        <f>COUNT(H2:H25)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1812</v>
       </c>
@@ -905,37 +828,8 @@
       <c r="G10">
         <v>834</v>
       </c>
-      <c r="H10">
-        <v>388</v>
-      </c>
-      <c r="I10">
-        <v>318</v>
-      </c>
-      <c r="K10">
-        <v>2013</v>
-      </c>
-      <c r="L10">
-        <f>AVERAGE(I2:I24)</f>
-        <v>384.43478260869563</v>
-      </c>
-      <c r="M10">
-        <f>MEDIAN(I2:I24)</f>
-        <v>395</v>
-      </c>
-      <c r="N10">
-        <f>MAX(I2:I24)</f>
-        <v>1054</v>
-      </c>
-      <c r="O10">
-        <f>MIN(I2:I24)</f>
-        <v>38</v>
-      </c>
-      <c r="P10">
-        <f>COUNT(I2:I24)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>780</v>
       </c>
@@ -957,14 +851,8 @@
       <c r="G11">
         <v>541</v>
       </c>
-      <c r="H11">
-        <v>447</v>
-      </c>
-      <c r="I11">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1620</v>
       </c>
@@ -986,14 +874,8 @@
       <c r="G12">
         <v>367</v>
       </c>
-      <c r="H12">
-        <v>1060</v>
-      </c>
-      <c r="I12">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1614</v>
       </c>
@@ -1015,14 +897,8 @@
       <c r="G13">
         <v>1318</v>
       </c>
-      <c r="H13">
-        <v>189</v>
-      </c>
-      <c r="I13">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1039</v>
       </c>
@@ -1044,14 +920,8 @@
       <c r="G14">
         <v>1609</v>
       </c>
-      <c r="H14">
-        <v>339</v>
-      </c>
-      <c r="I14">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>825</v>
       </c>
@@ -1073,14 +943,8 @@
       <c r="G15">
         <v>1044</v>
       </c>
-      <c r="H15">
-        <v>796</v>
-      </c>
-      <c r="I15">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1438</v>
       </c>
@@ -1102,14 +966,8 @@
       <c r="G16">
         <v>559</v>
       </c>
-      <c r="H16">
-        <v>209</v>
-      </c>
-      <c r="I16">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1163</v>
       </c>
@@ -1131,14 +989,8 @@
       <c r="G17">
         <v>791</v>
       </c>
-      <c r="H17">
-        <v>533</v>
-      </c>
-      <c r="I17">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>794</v>
       </c>
@@ -1160,14 +1012,8 @@
       <c r="G18">
         <v>520</v>
       </c>
-      <c r="H18">
-        <v>428</v>
-      </c>
-      <c r="I18">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>499</v>
       </c>
@@ -1186,14 +1032,8 @@
       <c r="G19">
         <v>780</v>
       </c>
-      <c r="H19">
-        <v>363</v>
-      </c>
-      <c r="I19">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1142</v>
       </c>
@@ -1212,14 +1052,8 @@
       <c r="G20">
         <v>1858</v>
       </c>
-      <c r="H20">
-        <v>486</v>
-      </c>
-      <c r="I20">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1277</v>
       </c>
@@ -1238,14 +1072,8 @@
       <c r="G21">
         <v>748</v>
       </c>
-      <c r="H21">
-        <v>71</v>
-      </c>
-      <c r="I21">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1782</v>
       </c>
@@ -1264,14 +1092,8 @@
       <c r="G22">
         <v>1175</v>
       </c>
-      <c r="H22">
-        <v>763</v>
-      </c>
-      <c r="I22">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>897</v>
       </c>
@@ -1287,14 +1109,8 @@
       <c r="G23">
         <v>731</v>
       </c>
-      <c r="H23">
-        <v>414</v>
-      </c>
-      <c r="I23">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>697</v>
       </c>
@@ -1304,14 +1120,8 @@
       <c r="F24">
         <v>701</v>
       </c>
-      <c r="H24">
-        <v>1221</v>
-      </c>
-      <c r="I24">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>561</v>
       </c>
@@ -1321,11 +1131,8 @@
       <c r="F25">
         <v>759</v>
       </c>
-      <c r="H25">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>670</v>
       </c>
@@ -1333,7 +1140,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>347</v>
       </c>
@@ -1341,27 +1148,27 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>1585</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>1029</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>673</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>614</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>1268</v>
       </c>

</xml_diff>